<commit_message>
change:   1. add table_details_draft   2. add mature table_details files   3. fix some bugs in outline doc(including change some nchar type to nvarchar types).
  ps: outline docs are deprecated now.Docs are always deprecated in later stage and would never update for improments and changes.So if you want to know about the latest status of the project,see the docs of latest stage.
</commit_message>
<xml_diff>
--- a/table details/table_details_1-8.xlsx
+++ b/table details/table_details_1-8.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D8BC08-7448-4590-85E5-ED3A3FCEC10A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AEDBE8-B3BA-4D23-8F78-C6541D5C4085}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-4" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="115">
   <si>
     <t>表名：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -464,6 +464,13 @@
   </si>
   <si>
     <t>jt_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nvarchar</t>
+  </si>
+  <si>
+    <t>nchar</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -822,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1303,7 +1310,7 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1312,9 +1319,6 @@
       </c>
       <c r="C29">
         <v>20</v>
-      </c>
-      <c r="D29">
-        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1367,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1417,7 +1421,7 @@
         <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1430,9 +1434,6 @@
       <c r="C5">
         <v>20</v>
       </c>
-      <c r="D5">
-        <v>100</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1503,7 +1504,7 @@
         <v>37</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1513,9 +1514,6 @@
       <c r="C13">
         <v>20</v>
       </c>
-      <c r="D13">
-        <v>100</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -1675,7 +1673,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>37</v>
+        <v>114</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>37</v>
@@ -1687,9 +1685,6 @@
       </c>
       <c r="C29">
         <v>10</v>
-      </c>
-      <c r="D29">
-        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
finish power designer work
1. finish power designer work(cdm,ldm,pdm,sql)
2. modify part of doc and table_details excel
</commit_message>
<xml_diff>
--- a/table details/table_details_1-8.xlsx
+++ b/table details/table_details_1-8.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AEDBE8-B3BA-4D23-8F78-C6541D5C4085}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BAFBF3-919B-4E91-ADBD-AC1AE547A5E7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-4" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="122">
   <si>
     <t>表名：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,10 +74,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>招聘人数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -106,22 +102,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>姓名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>年龄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>性别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>职位id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -138,26 +118,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>工作地点id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>职能类别id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>职能类别描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>紧急度id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>职位id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>职位描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -171,10 +135,6 @@
     <t>nchar</t>
   </si>
   <si>
-    <t>Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -216,18 +176,10 @@
     <t>smallint</t>
   </si>
   <si>
-    <t>rr_dpt_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>rr_wp_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>rr_wk_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>rr_st_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -272,10 +224,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>requirements_info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>部门id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -320,22 +268,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>stf_role_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>密码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>权限id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ri_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -352,10 +284,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ri_spreq</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ntext</t>
   </si>
   <si>
@@ -471,6 +399,105 @@
   </si>
   <si>
     <t>nchar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nvarchar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tinyint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stf_email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>requirements_common_info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职员id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职员姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职员年龄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职员性别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职员职位id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职员用户名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职员密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职员邮箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>smalldatetime</t>
+  </si>
+  <si>
+    <t>招聘需求id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>积分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stf_pts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职员电话</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职员部门id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stf_tel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stf_dp_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ri_dpt_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ri_wk_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rr_spreq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nvarchar</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -829,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -841,6 +868,8 @@
     <col min="5" max="5" width="11.125" customWidth="1"/>
     <col min="6" max="6" width="11.375" customWidth="1"/>
     <col min="7" max="7" width="10.75" customWidth="1"/>
+    <col min="8" max="8" width="13.25" customWidth="1"/>
+    <col min="10" max="10" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -853,10 +882,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -864,37 +893,34 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>65</v>
-      </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -902,44 +928,41 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5">
+      <c r="F5">
         <v>20</v>
       </c>
     </row>
@@ -948,37 +971,34 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -986,37 +1006,34 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="K7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1029,10 +1046,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1040,28 +1057,37 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="G11" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="I11" t="s">
-        <v>79</v>
+        <v>109</v>
+      </c>
+      <c r="J11" t="s">
+        <v>112</v>
+      </c>
+      <c r="K11" t="s">
+        <v>114</v>
+      </c>
+      <c r="L11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1069,28 +1095,37 @@
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1101,12 +1136,18 @@
         <v>20</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>20</v>
       </c>
       <c r="H13">
+        <v>20</v>
+      </c>
+      <c r="I13">
+        <v>20</v>
+      </c>
+      <c r="K13">
         <v>20</v>
       </c>
     </row>
@@ -1115,28 +1156,37 @@
         <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>45</v>
+        <v>99</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1144,132 +1194,153 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="G15" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="H15" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="I15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="J15" t="s">
+        <v>113</v>
+      </c>
+      <c r="K15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="G23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1277,29 +1348,29 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -1307,13 +1378,13 @@
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -1321,45 +1392,48 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:L6 B14:I14 B30 B22:F22" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:L14 B30 B6:K6 B22:G22" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"k,m,k&amp;m,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28:D28 B4:L4 B12:I12 B20:F20" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28:D28 B12:L12 B20:G20 B4:E4 G4:K4" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30:D30" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"k,m,k&amp;m"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{A0B6BE8E-FC8B-471C-84BE-24CFF94A9FEA}">
+      <formula1>"tinyint,smallint,int,nchar,nvarchar,ntext,smalldatetime"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1371,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1390,10 +1464,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1401,13 +1475,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1415,22 +1489,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
       <c r="C5">
         <v>20</v>
       </c>
@@ -1440,13 +1511,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1454,13 +1525,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1473,10 +1544,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1484,13 +1555,13 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1501,10 +1572,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1520,13 +1591,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1534,13 +1605,13 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1553,10 +1624,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1564,16 +1635,16 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
         <v>34</v>
-      </c>
-      <c r="E19" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1581,16 +1652,16 @@
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1606,16 +1677,16 @@
         <v>6</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1623,32 +1694,32 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="E23" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1656,13 +1727,13 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1670,13 +1741,13 @@
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1692,13 +1763,13 @@
         <v>6</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1706,13 +1777,13 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>